<commit_message>
= que me falto en for de excel quitar comentario a login
</commit_message>
<xml_diff>
--- a/Ventas/ExcelDB/Database.xlsx
+++ b/Ventas/ExcelDB/Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\source\repos\VentasDB-master-CLASE\Ventas\ExcelDB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\source\repos\Ventas-jd\Ventas\ExcelDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78342E1E-9FFC-4AA6-93DC-FFE19A3B8C89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2315ED2D-C6DF-4266-8126-79EAE51F823E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EMPLEADOS" sheetId="2" r:id="rId1"/>
@@ -468,7 +468,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,6 +511,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Clases y funciones, CRUD
</commit_message>
<xml_diff>
--- a/Ventas/ExcelDB/Database.xlsx
+++ b/Ventas/ExcelDB/Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\source\repos\Ventas-jd\Ventas\ExcelDB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2315ED2D-C6DF-4266-8126-79EAE51F823E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{704232EB-D43D-402B-ABB1-1E1EA27080AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29265" yWindow="705" windowWidth="28635" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EMPLEADOS" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="64">
   <si>
     <t>Id</t>
   </si>
@@ -89,6 +89,138 @@
   </si>
   <si>
     <t>Jose Dyck</t>
+  </si>
+  <si>
+    <t>Electronicos</t>
+  </si>
+  <si>
+    <t>Equipos Electronicos</t>
+  </si>
+  <si>
+    <t>Comestibles</t>
+  </si>
+  <si>
+    <t>Todo tipo de comestibles</t>
+  </si>
+  <si>
+    <t>Bebidas</t>
+  </si>
+  <si>
+    <t>Todo tipo de bebidas</t>
+  </si>
+  <si>
+    <t>Empaquetados</t>
+  </si>
+  <si>
+    <t>Producto en paquete</t>
+  </si>
+  <si>
+    <t>A granel</t>
+  </si>
+  <si>
+    <t>Producto venta a granel</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>Productos que no pueden venderse por si solos</t>
+  </si>
+  <si>
+    <t>Enlatados</t>
+  </si>
+  <si>
+    <t>Productos en lata</t>
+  </si>
+  <si>
+    <t>Reposteria</t>
+  </si>
+  <si>
+    <t>Productos de reposteria</t>
+  </si>
+  <si>
+    <t>Carniceria</t>
+  </si>
+  <si>
+    <t>Res, puerco y ternera</t>
+  </si>
+  <si>
+    <t>Pescaderia</t>
+  </si>
+  <si>
+    <t>Productos del mar</t>
+  </si>
+  <si>
+    <t>Especias</t>
+  </si>
+  <si>
+    <t>Todo tipo de especias</t>
+  </si>
+  <si>
+    <t>Verduras</t>
+  </si>
+  <si>
+    <t>Todo tipo de verduras</t>
+  </si>
+  <si>
+    <t>Lacteos</t>
+  </si>
+  <si>
+    <t>Todo tipo de lacteos</t>
+  </si>
+  <si>
+    <t>Carnes frias</t>
+  </si>
+  <si>
+    <t>Embutidos y carnes frias</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>desde excel</t>
+  </si>
+  <si>
+    <t>Agua ciel de 1 LT</t>
+  </si>
+  <si>
+    <t>e Pura 600 ml</t>
+  </si>
+  <si>
+    <t>Coca Cola 1 LT</t>
+  </si>
+  <si>
+    <t>Nutrileche 1 Lt</t>
+  </si>
+  <si>
+    <t>Lechuga Romana</t>
+  </si>
+  <si>
+    <t>Aguacate Kg</t>
+  </si>
+  <si>
+    <t>Sal de mesa 1 Kg</t>
+  </si>
+  <si>
+    <t>AZUCAR ZULCA 1KG</t>
+  </si>
+  <si>
+    <t>CUBO KNORR DE POLLO</t>
+  </si>
+  <si>
+    <t>ACEITE CRISTAL</t>
+  </si>
+  <si>
+    <t>Astral del Pacifico SA de CV.</t>
+  </si>
+  <si>
+    <t>Coca Cola SA de CV</t>
+  </si>
+  <si>
+    <t>Grupo Bimbo SA de CV</t>
+  </si>
+  <si>
+    <t>Sabritas SA de CV.-favorito</t>
   </si>
 </sst>
 </file>
@@ -124,9 +256,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15E722B6-26AE-4635-B99A-D655BAF05612}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,6 +644,17 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -517,19 +663,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35D74FA8-95FD-446E-B3E2-79E5BE4AAD6E}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -541,6 +687,160 @@
       </c>
       <c r="D1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="2">
+        <v>16.5</v>
+      </c>
+      <c r="D2" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" s="2">
+        <v>8</v>
+      </c>
+      <c r="D3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" s="2">
+        <v>15</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" s="2">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="2">
+        <v>15</v>
+      </c>
+      <c r="D6" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="2">
+        <v>35</v>
+      </c>
+      <c r="D7" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="2">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" s="2">
+        <v>25</v>
+      </c>
+      <c r="D9" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="2">
+        <v>5</v>
+      </c>
+      <c r="D10" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="2">
+        <v>30</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="2">
+        <v>1</v>
+      </c>
+      <c r="D12" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -551,15 +851,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{500EA8A8-AF56-4DCE-B6F1-42FEAE9C27AD}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="25.85546875" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -568,6 +868,38 @@
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -577,18 +909,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46FD07F-BA48-47A0-B72B-6995ECC68DA6}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="22.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -597,6 +930,171 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>